<commit_message>
Change getMarkLines help output
</commit_message>
<xml_diff>
--- a/assign1/all-1.xlsx
+++ b/assign1/all-1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,21 +16,7 @@
     <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$F$2:$F$131</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$G$1</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$G$2:$G$131</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$131</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$B$2:$B$131</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$C$2:$C$131</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$D$2:$D$131</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$E$2:$E$131</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$F$2:$F$131</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$G$2:$G$131</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$131</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$131</definedName>
@@ -859,10 +845,10 @@
       <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>532834</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>51261</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -898,8 +884,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5490881" y="195261"/>
-              <a:ext cx="13406719" cy="9348789"/>
+              <a:off x="5450540" y="195261"/>
+              <a:ext cx="9000000" cy="9000000"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1198,7 +1184,7 @@
   <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>